<commit_message>
se agrego la funcionabildad de las graficas en el excel, se mejoraron algunos procesos, se agrego el slider de porcentaje de avance.
</commit_message>
<xml_diff>
--- a/personas.xlsx
+++ b/personas.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>CODIGO</t>
   </si>
@@ -41,13 +41,22 @@
     <t>Base de Datos</t>
   </si>
   <si>
-    <t>P004</t>
+    <t>P005</t>
   </si>
   <si>
     <t>Esteban Cardenas</t>
   </si>
   <si>
     <t>Desarrollador Backend</t>
+  </si>
+  <si>
+    <t>P007</t>
+  </si>
+  <si>
+    <t>Thiago Isaac</t>
+  </si>
+  <si>
+    <t>Arquitecto de Software</t>
   </si>
 </sst>
 </file>
@@ -92,7 +101,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -100,7 +109,7 @@
   <cols>
     <col min="1" max="1" width="8.41796875" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="16.98046875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="21.32421875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="21.8671875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -147,6 +156,17 @@
         <v>11</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>